<commit_message>
overcome a problem in Tranf2TimeDomain. Missing a .copy()
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AQ66740\OneDrive - ETS\Desktop\New folder\Prony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{5E44D781-A510-41A7-837F-0F78A56B2B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{53A9FA84-2A5E-49BF-A603-91B055A447FB}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{5E44D781-A510-41A7-837F-0F78A56B2B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B749F346-D717-4E1F-83D9-F11B964AB0DA}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{E56D9212-0D79-4365-86CB-5BA71332F209}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{E56D9212-0D79-4365-86CB-5BA71332F209}"/>
   </bookViews>
   <sheets>
     <sheet name="180" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -402,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A0FE74-9D05-4A49-9AE8-F18C99A19A44}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +558,7 @@
         <v>0.67800000000000005</v>
       </c>
       <c r="B15" s="2">
-        <v>4.71</v>
+        <v>4.51</v>
       </c>
       <c r="C15" s="2">
         <v>406</v>
@@ -578,7 +569,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="B16" s="2">
-        <v>2.46</v>
+        <v>1.86</v>
       </c>
       <c r="C16" s="2">
         <v>252</v>
@@ -589,7 +580,7 @@
         <v>0.26600000000000001</v>
       </c>
       <c r="B17" s="2">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="C17" s="2">
         <v>155</v>
@@ -613,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CD5547-12F4-42D4-B4BC-DBC92F2CAC3C}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +791,7 @@
         <v>0.26600000000000001</v>
       </c>
       <c r="B17" s="2">
-        <v>4.43</v>
+        <v>3.43</v>
       </c>
       <c r="C17" s="2">
         <v>385</v>
@@ -1060,16 +1051,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0105C5BB-91F9-4603-9C3E-24499947A68A}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00f5968f-c960-4f77-8272-392e3a2178b6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="04e0ef68-9bf3-4219-b454-cda4eb54df8d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="04e0ef68-9bf3-4219-b454-cda4eb54df8d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00f5968f-c960-4f77-8272-392e3a2178b6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
frequency written in hz and not in rad/s
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AQ66740\OneDrive - ETS\Desktop\New folder\Prony\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\PRONY\Prony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{5E44D781-A510-41A7-837F-0F78A56B2B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B749F346-D717-4E1F-83D9-F11B964AB0DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA239943-4F36-44EF-B173-317955372091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{E56D9212-0D79-4365-86CB-5BA71332F209}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E56D9212-0D79-4365-86CB-5BA71332F209}"/>
   </bookViews>
   <sheets>
     <sheet name="180" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -393,13 +402,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A0FE74-9D05-4A49-9AE8-F18C99A19A44}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,9 +419,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>300</v>
+        <v>47.7464829275686</v>
       </c>
       <c r="B2" s="2">
         <v>53700</v>
@@ -421,9 +430,9 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>188</v>
+        <v>29.921129301276324</v>
       </c>
       <c r="B3" s="2">
         <v>33600</v>
@@ -432,9 +441,9 @@
         <v>64900</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>118</v>
+        <v>18.780283284843652</v>
       </c>
       <c r="B4" s="2">
         <v>19900</v>
@@ -443,9 +452,9 @@
         <v>47800</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>73.599999999999994</v>
+        <v>11.713803811563496</v>
       </c>
       <c r="B5" s="2">
         <v>11200</v>
@@ -454,9 +463,9 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>46</v>
+        <v>7.3211273822271856</v>
       </c>
       <c r="B6" s="2">
         <v>5960</v>
@@ -465,9 +474,9 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>28.8</v>
+        <v>4.5836623610465859</v>
       </c>
       <c r="B7" s="2">
         <v>3020</v>
@@ -476,9 +485,9 @@
         <v>15800</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>18</v>
+        <v>2.8647889756541161</v>
       </c>
       <c r="B8" s="2">
         <v>1450</v>
@@ -487,9 +496,9 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>11.3</v>
+        <v>1.7984508569384174</v>
       </c>
       <c r="B9" s="2">
         <v>667</v>
@@ -498,9 +507,9 @@
         <v>6570</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>7.06</v>
+        <v>1.123633898228781</v>
       </c>
       <c r="B10" s="2">
         <v>298</v>
@@ -509,9 +518,9 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4.42</v>
+        <v>0.70346484846617741</v>
       </c>
       <c r="B11" s="2">
         <v>129</v>
@@ -520,9 +529,9 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2.77</v>
+        <v>0.44085919236455012</v>
       </c>
       <c r="B12" s="2">
         <v>55.9</v>
@@ -531,9 +540,9 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1.73</v>
+        <v>0.27533805154897895</v>
       </c>
       <c r="B13" s="2">
         <v>24.4</v>
@@ -542,9 +551,9 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1.08</v>
+        <v>0.17188733853924698</v>
       </c>
       <c r="B14" s="2">
         <v>10.9</v>
@@ -553,9 +562,9 @@
         <v>650</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.67800000000000005</v>
+        <v>0.10790705141630505</v>
       </c>
       <c r="B15" s="2">
         <v>4.51</v>
@@ -564,9 +573,9 @@
         <v>406</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.42499999999999999</v>
+        <v>6.764085081405552E-2</v>
       </c>
       <c r="B16" s="2">
         <v>1.86</v>
@@ -575,9 +584,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.26600000000000001</v>
+        <v>4.2335214862444161E-2</v>
       </c>
       <c r="B17" s="2">
         <v>0.75</v>
@@ -586,11 +595,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -604,13 +613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CD5547-12F4-42D4-B4BC-DBC92F2CAC3C}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,9 +630,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>300</v>
+        <v>47.7464829275686</v>
       </c>
       <c r="B2" s="2">
         <v>112000</v>
@@ -632,9 +641,9 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>188</v>
+        <v>29.921129301276324</v>
       </c>
       <c r="B3" s="2">
         <v>76900</v>
@@ -643,9 +652,9 @@
         <v>103000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>118</v>
+        <v>18.780283284843652</v>
       </c>
       <c r="B4" s="2">
         <v>50700</v>
@@ -654,9 +663,9 @@
         <v>82000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>73.599999999999994</v>
+        <v>11.713803811563496</v>
       </c>
       <c r="B5" s="2">
         <v>31700</v>
@@ -665,9 +674,9 @@
         <v>62500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>46</v>
+        <v>7.3211273822271856</v>
       </c>
       <c r="B6" s="2">
         <v>18700</v>
@@ -676,9 +685,9 @@
         <v>45900</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>28.8</v>
+        <v>4.5836623610465859</v>
       </c>
       <c r="B7" s="2">
         <v>10500</v>
@@ -687,9 +696,9 @@
         <v>32800</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>18</v>
+        <v>2.8647889756541161</v>
       </c>
       <c r="B8" s="2">
         <v>5450</v>
@@ -698,9 +707,9 @@
         <v>22300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>11.3</v>
+        <v>1.7984508569384174</v>
       </c>
       <c r="B9" s="2">
         <v>2700</v>
@@ -709,9 +718,9 @@
         <v>14900</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>7.06</v>
+        <v>1.123633898228781</v>
       </c>
       <c r="B10" s="2">
         <v>1270</v>
@@ -720,9 +729,9 @@
         <v>9720</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4.42</v>
+        <v>0.70346484846617741</v>
       </c>
       <c r="B11" s="2">
         <v>567</v>
@@ -731,9 +740,9 @@
         <v>6240</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2.77</v>
+        <v>0.44085919236455012</v>
       </c>
       <c r="B12" s="2">
         <v>244</v>
@@ -742,9 +751,9 @@
         <v>3970</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1.73</v>
+        <v>0.27533805154897895</v>
       </c>
       <c r="B13" s="2">
         <v>102</v>
@@ -753,9 +762,9 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1.08</v>
+        <v>0.17188733853924698</v>
       </c>
       <c r="B14" s="2">
         <v>43.6</v>
@@ -764,9 +773,9 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.67800000000000005</v>
+        <v>0.10790705141630505</v>
       </c>
       <c r="B15" s="2">
         <v>20.3</v>
@@ -775,9 +784,9 @@
         <v>990</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.42499999999999999</v>
+        <v>6.764085081405552E-2</v>
       </c>
       <c r="B16" s="2">
         <v>7.89</v>
@@ -786,9 +795,9 @@
         <v>618</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.26600000000000001</v>
+        <v>4.2335214862444161E-2</v>
       </c>
       <c r="B17" s="2">
         <v>3.43</v>
@@ -797,11 +806,11 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
@@ -817,15 +826,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000019EA7267B4C44C8D7AFFEC7F14AA2C" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1261eb3d9fc2108fedc05446de713b55">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="00f5968f-c960-4f77-8272-392e3a2178b6" xmlns:ns4="04e0ef68-9bf3-4219-b454-cda4eb54df8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3269ec9219913036074ac431cb0f1464" ns3:_="" ns4:_="">
     <xsd:import namespace="00f5968f-c960-4f77-8272-392e3a2178b6"/>
@@ -1048,6 +1048,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0105C5BB-91F9-4603-9C3E-24499947A68A}">
   <ds:schemaRefs>
@@ -1066,14 +1075,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51E5B9CB-C480-4FCC-BDBC-EEF63294C0D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C86059-4713-452C-BA45-6F0752E1A3D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1090,4 +1091,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51E5B9CB-C480-4FCC-BDBC-EEF63294C0D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>